<commit_message>
4.1 Xoá vĩnh viễn
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAB2449-4EA5-4189-A487-17A021842E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6242A7C0-1ECF-430B-AA9A-52F33E1C6ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/262d8a2429fc1cdc879187949eea553f2f23143c</t>
+  </si>
+  <si>
+    <t>3.2. Thay đổi trạng thái nhiều sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/e896019a677ede65944dae61c70a40c4ecc8a67d</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +466,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A65D3D43-F78C-41D3-8A84-11E38DC0B1B8}"/>

</xml_diff>

<commit_message>
1. Xoá nhiều sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897B697-A1D4-4555-AF1E-B031D3508338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B2E44B-9186-4F6B-8C1C-CA8139799AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <t>4.2 Xoá mềm</t>
   </si>
   <si>
-    <t>https://github.com/nguyentienminh07102004/product-management/commit/bb0ab7d3374d7dd08cd24dce9d83f6b61bb7f218</t>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/41534278856704293c82600456b1f6467babb5b8</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -507,6 +507,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A65D3D43-F78C-41D3-8A84-11E38DC0B1B8}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{629FC09C-13EB-4D1E-B909-FA910E6A199D}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{15C11790-4A80-420B-9452-E8A3FDEACE88}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{E94B4021-9A53-4611-A752-FC3640886A41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2. Tính năng thay đổi thứ tự sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B2E44B-9186-4F6B-8C1C-CA8139799AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E05D8C-69B8-4D8C-8D19-5581E96651A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/41534278856704293c82600456b1f6467babb5b8</t>
+  </si>
+  <si>
+    <t>Bài 18</t>
+  </si>
+  <si>
+    <t>1. Xoá nhiều sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/23586a985d09cd41448981b336656f09c95dd7dd</t>
   </si>
 </sst>
 </file>
@@ -435,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,12 +511,24 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A65D3D43-F78C-41D3-8A84-11E38DC0B1B8}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{629FC09C-13EB-4D1E-B909-FA910E6A199D}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{15C11790-4A80-420B-9452-E8A3FDEACE88}"/>
     <hyperlink ref="C6" r:id="rId4" xr:uid="{E94B4021-9A53-4611-A752-FC3640886A41}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{B4E48B36-7521-4857-8BBB-9A3D98531B44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3.1. Hiển thị thông báo sau khi đổi trạng thái
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E05D8C-69B8-4D8C-8D19-5581E96651A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC93DE26-5427-4C57-9EBD-3E07033B5D98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/23586a985d09cd41448981b336656f09c95dd7dd</t>
+  </si>
+  <si>
+    <t>2. Tính năng thay đổi thứ tự sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/a36764f2bc798b74ffb3bdda7168d990212f567d</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,14 +127,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,57 +491,70 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -529,6 +564,7 @@
     <hyperlink ref="C5" r:id="rId3" xr:uid="{15C11790-4A80-420B-9452-E8A3FDEACE88}"/>
     <hyperlink ref="C6" r:id="rId4" xr:uid="{E94B4021-9A53-4611-A752-FC3640886A41}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{B4E48B36-7521-4857-8BBB-9A3D98531B44}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{0790A294-F4BE-455E-9096-556D9F5A12F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3.2. Hiển thị thông báo sau khi xóa
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC93DE26-5427-4C57-9EBD-3E07033B5D98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF1FF40-2AD3-47B3-9A1C-F998B769C0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/a36764f2bc798b74ffb3bdda7168d990212f567d</t>
+  </si>
+  <si>
+    <t>3.1. Hiển thị thông báo sau khi đổi trạng thái</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/e72573281984dbf2b78af3ac8215ef1773f841a9</t>
   </si>
 </sst>
 </file>
@@ -466,16 +472,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" activeCellId="8" sqref="C2 C3 C4 C5 C6 C7 C8 C9 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="225.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -515,7 +521,7 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -555,6 +561,15 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -565,6 +580,8 @@
     <hyperlink ref="C6" r:id="rId4" xr:uid="{E94B4021-9A53-4611-A752-FC3640886A41}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{B4E48B36-7521-4857-8BBB-9A3D98531B44}"/>
     <hyperlink ref="C8" r:id="rId6" xr:uid="{0790A294-F4BE-455E-9096-556D9F5A12F2}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{884F90D0-F97A-47D7-B300-B42973604977}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{0E505A28-9D53-4DF2-A60C-1E056F75FC97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3.3. Hiển thị thông báo sau khi đổi vị trí
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF1FF40-2AD3-47B3-9A1C-F998B769C0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01FB4E7-C05A-4154-93F5-C2678E310386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/e72573281984dbf2b78af3ac8215ef1773f841a9</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/9516b17e3bbe0f9823dc17f0bdf0c65b8008935b</t>
+  </si>
+  <si>
+    <t>3.2. Hiển thị thông báo sau khi xóa</t>
   </si>
 </sst>
 </file>
@@ -153,10 +159,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" activeCellId="8" sqref="C2 C3 C4 C5 C6 C7 C8 C9 C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +579,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A65D3D43-F78C-41D3-8A84-11E38DC0B1B8}"/>
@@ -582,6 +597,7 @@
     <hyperlink ref="C8" r:id="rId6" xr:uid="{0790A294-F4BE-455E-9096-556D9F5A12F2}"/>
     <hyperlink ref="C9" r:id="rId7" xr:uid="{884F90D0-F97A-47D7-B300-B42973604977}"/>
     <hyperlink ref="C4" r:id="rId8" xr:uid="{0E505A28-9D53-4DF2-A60C-1E056F75FC97}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{821476D5-1F55-425E-AB1E-DE7A88ACF06E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
4. Tính năng tạo mới sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01FB4E7-C05A-4154-93F5-C2678E310386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67588E-9D04-48DC-AA4D-D4F3002DB080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>3.2. Hiển thị thông báo sau khi xóa</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/6cacbdd5ab0f00482423975c4dfea365d3835ef6</t>
+  </si>
+  <si>
+    <t>3.3. Hiển thị thông báo sau khi đổi vị trí</t>
+  </si>
+  <si>
+    <t>4. Tính năng tạo mới sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -123,12 +132,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -159,11 +174,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,41 +570,58 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -598,7 +634,9 @@
     <hyperlink ref="C9" r:id="rId7" xr:uid="{884F90D0-F97A-47D7-B300-B42973604977}"/>
     <hyperlink ref="C4" r:id="rId8" xr:uid="{0E505A28-9D53-4DF2-A60C-1E056F75FC97}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{821476D5-1F55-425E-AB1E-DE7A88ACF06E}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{5984C680-31CD-44E9-8333-C144150AD239}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4. Tạo mới sản phẩm có upload ảnh chưa có preview ảnh khi upoad
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67588E-9D04-48DC-AA4D-D4F3002DB080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49109E3-512D-477F-9694-A6FCA8A95688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -66,9 +66,6 @@
     <t>4.1. Xóa vĩnh viễn</t>
   </si>
   <si>
-    <t>https://githttps://github.com/nguyentienminh07102004/product-management/commit/f1ac942243f94ace9433ec5239d0ec416202bf6bhub.com/nguyentienminh07102004/product-management/commit/f1ac942243f94ace9433ec5239d0ec416202bf6b</t>
-  </si>
-  <si>
     <t>4.2 Xoá mềm</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>4. Tính năng tạo mới sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/a4a024e0a5282e29b9c0298532c0093a1674ed60</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/f1ac942243f94ace9433ec5239d0ec416202bf6b</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -183,6 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +505,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,71 +561,73 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -635,8 +641,9 @@
     <hyperlink ref="C4" r:id="rId8" xr:uid="{0E505A28-9D53-4DF2-A60C-1E056F75FC97}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{821476D5-1F55-425E-AB1E-DE7A88ACF06E}"/>
     <hyperlink ref="C11" r:id="rId10" xr:uid="{5984C680-31CD-44E9-8333-C144150AD239}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{0750AE1E-F7B7-472A-98DE-F922DA3E206A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2.Tính năng chỉnh sửa sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC21042D-10A7-46E3-B53A-A79246F42727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719C52B-CFBE-435A-941A-0A5E9A75AE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Sửa lỗi hàm sort() và preview ảnh sau khi upload</t>
+  </si>
+  <si>
+    <t>Bài19</t>
+  </si>
+  <si>
+    <t>1. Validate dữ liệu</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/c718b5b12a9cfe129b0fd827888980b0087cc7d7</t>
   </si>
 </sst>
 </file>
@@ -183,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -193,6 +202,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -508,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +651,17 @@
       </c>
       <c r="C13" s="3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -657,8 +678,9 @@
     <hyperlink ref="C11" r:id="rId10" xr:uid="{5984C680-31CD-44E9-8333-C144150AD239}"/>
     <hyperlink ref="C12" r:id="rId11" xr:uid="{0750AE1E-F7B7-472A-98DE-F922DA3E206A}"/>
     <hyperlink ref="C13" r:id="rId12" location="diff-68bb4443c78a25e82cde57e42b44964d10cf5cd8e4878332c7776fe1a34ef3a0" xr:uid="{5C548DF3-506D-4B63-8E5F-C1E2E9ADFBD0}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{9DF701D7-4CF2-4846-B791-5BF607FCDCF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3. Làm trang chi tiết sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719C52B-CFBE-435A-941A-0A5E9A75AE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D79AA-59C6-412F-BC5C-2FECC8C5A57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/c718b5b12a9cfe129b0fd827888980b0087cc7d7</t>
+  </si>
+  <si>
+    <t>2.Tính năng chỉnh sửa sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/70880148cb582135eeaf8cec827259f7c0d96679</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,6 +668,14 @@
       </c>
       <c r="C14" s="9" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -679,8 +693,9 @@
     <hyperlink ref="C12" r:id="rId11" xr:uid="{0750AE1E-F7B7-472A-98DE-F922DA3E206A}"/>
     <hyperlink ref="C13" r:id="rId12" location="diff-68bb4443c78a25e82cde57e42b44964d10cf5cd8e4878332c7776fe1a34ef3a0" xr:uid="{5C548DF3-506D-4B63-8E5F-C1E2E9ADFBD0}"/>
     <hyperlink ref="C14" r:id="rId13" xr:uid="{9DF701D7-4CF2-4846-B791-5BF607FCDCF0}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{22C6849D-477A-4245-8799-99750A50DFB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4. Làm trang chi tiết sản phẩm phía client
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D79AA-59C6-412F-BC5C-2FECC8C5A57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185067EE-8537-464F-889E-F8B089A33C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -133,13 +133,25 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/70880148cb582135eeaf8cec827259f7c0d96679</t>
+  </si>
+  <si>
+    <t>3. Làm trang chi tiết sản phẩm</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/983e0d92ab7d9e289e7960222c56191726c9ee3b</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/29f18558b986394d081660cdb829085dff440671</t>
+  </si>
+  <si>
+    <t>4. Tính năng tạo mới sản phẩm(Có upload ảnh chưa có preview)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +167,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +184,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -208,7 +238,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,17 +562,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="225.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="184.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,33 +690,78 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="17"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A65D3D43-F78C-41D3-8A84-11E38DC0B1B8}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{629FC09C-13EB-4D1E-B909-FA910E6A199D}"/>
@@ -691,11 +774,13 @@
     <hyperlink ref="C10" r:id="rId9" xr:uid="{821476D5-1F55-425E-AB1E-DE7A88ACF06E}"/>
     <hyperlink ref="C11" r:id="rId10" xr:uid="{5984C680-31CD-44E9-8333-C144150AD239}"/>
     <hyperlink ref="C12" r:id="rId11" xr:uid="{0750AE1E-F7B7-472A-98DE-F922DA3E206A}"/>
-    <hyperlink ref="C13" r:id="rId12" location="diff-68bb4443c78a25e82cde57e42b44964d10cf5cd8e4878332c7776fe1a34ef3a0" xr:uid="{5C548DF3-506D-4B63-8E5F-C1E2E9ADFBD0}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{9DF701D7-4CF2-4846-B791-5BF607FCDCF0}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{22C6849D-477A-4245-8799-99750A50DFB8}"/>
+    <hyperlink ref="C14" r:id="rId12" location="diff-68bb4443c78a25e82cde57e42b44964d10cf5cd8e4878332c7776fe1a34ef3a0" xr:uid="{5C548DF3-506D-4B63-8E5F-C1E2E9ADFBD0}"/>
+    <hyperlink ref="C15" r:id="rId13" xr:uid="{9DF701D7-4CF2-4846-B791-5BF607FCDCF0}"/>
+    <hyperlink ref="C16" r:id="rId14" xr:uid="{22C6849D-477A-4245-8799-99750A50DFB8}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{8EC07181-B5C3-4E06-8F6A-9F5C969D3F9D}"/>
+    <hyperlink ref="C13" r:id="rId16" xr:uid="{553A3170-41BE-491C-BCA2-C19D459F7910}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
5.2 Đẩy code lên trên vercel
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4C2779-4DE3-49C6-B873-CD325D657F35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B315D58-BC08-49D3-A6DC-5BE2C96EDC76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/5351de16fa44104a986d26dc08267518f184a914</t>
+  </si>
+  <si>
+    <t>5.1. MongoDB Atlas</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/558d759eeb8d271edd366b6f9c1191d0dca0397e</t>
   </si>
 </sst>
 </file>
@@ -251,8 +257,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -571,7 +577,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,8 +763,12 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -768,7 +778,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -790,8 +800,9 @@
     <hyperlink ref="C17" r:id="rId15" xr:uid="{8EC07181-B5C3-4E06-8F6A-9F5C969D3F9D}"/>
     <hyperlink ref="C13" r:id="rId16" xr:uid="{553A3170-41BE-491C-BCA2-C19D459F7910}"/>
     <hyperlink ref="C18" r:id="rId17" xr:uid="{B9BA2D56-A40D-4C16-9D2F-B92CEA5DAAAB}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{2248F79B-D5C3-4DD7-A914-647B899D1A17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Sắp xếp sản phẩm theo các tiêu chí khác nhau
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358C1059-E755-49CA-85AB-D0B0DDE96B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A34DD-BA5C-4A7B-98CE-9C9031E853DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/02f8aea1e0db571fbed87613c59be8d72d5a99b2</t>
+  </si>
+  <si>
+    <t>6. Đẩy file tĩnh lên trên cloud</t>
+  </si>
+  <si>
+    <t>https://github.com/nguyentienminh07102004/product-management/commit/40564ed629ff1085a1e16ddb2c9fdef618240676</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -262,7 +268,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -581,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +776,7 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -780,14 +785,18 @@
       <c r="B20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -811,8 +820,9 @@
     <hyperlink ref="C18" r:id="rId17" xr:uid="{B9BA2D56-A40D-4C16-9D2F-B92CEA5DAAAB}"/>
     <hyperlink ref="C19" r:id="rId18" xr:uid="{2248F79B-D5C3-4DD7-A914-647B899D1A17}"/>
     <hyperlink ref="C20" r:id="rId19" xr:uid="{17C9D44D-C66A-4741-AE74-71BEFB321375}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{E01490D7-8388-4F9D-83AD-E22DFD5AA4CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2. tiny MCE base
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A34DD-BA5C-4A7B-98CE-9C9031E853DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30923C9-0F9D-4BA9-A011-F901725EE533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>https://github.com/nguyentienminh07102004/product-management/commit/40564ed629ff1085a1e16ddb2c9fdef618240676</t>
+  </si>
+  <si>
+    <t>Bài 20</t>
+  </si>
+  <si>
+    <t>1. Sắp xếp sản phẩm theo các tiêu chí khác nhau</t>
   </si>
 </sst>
 </file>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,6 +802,14 @@
       </c>
       <c r="C21" s="15" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -821,8 +835,9 @@
     <hyperlink ref="C19" r:id="rId18" xr:uid="{2248F79B-D5C3-4DD7-A914-647B899D1A17}"/>
     <hyperlink ref="C20" r:id="rId19" xr:uid="{17C9D44D-C66A-4741-AE74-71BEFB321375}"/>
     <hyperlink ref="C21" r:id="rId20" xr:uid="{E01490D7-8388-4F9D-83AD-E22DFD5AA4CA}"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://github.com/nguyentienminh07102004/product-management/commit/d0a373564e97957e32fc6716531b8809e75cba35" xr:uid="{CA423CC0-9546-4B5B-B690-3C96F405BB13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3. Danh mục sản phẩm
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30923C9-0F9D-4BA9-A011-F901725EE533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB0AFD1-1951-4301-953C-D327543BD85E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>1. Sắp xếp sản phẩm theo các tiêu chí khác nhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. tiny MCE base </t>
   </si>
 </sst>
 </file>
@@ -590,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +813,11 @@
       </c>
       <c r="B22" s="15" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -836,8 +844,9 @@
     <hyperlink ref="C20" r:id="rId19" xr:uid="{17C9D44D-C66A-4741-AE74-71BEFB321375}"/>
     <hyperlink ref="C21" r:id="rId20" xr:uid="{E01490D7-8388-4F9D-83AD-E22DFD5AA4CA}"/>
     <hyperlink ref="B22" r:id="rId21" display="https://github.com/nguyentienminh07102004/product-management/commit/d0a373564e97957e32fc6716531b8809e75cba35" xr:uid="{CA423CC0-9546-4B5B-B690-3C96F405BB13}"/>
+    <hyperlink ref="B23" r:id="rId22" location="diff-4ea027d01c6e49507fa3f91d5a63f7466ff135dff36912874b4cf40bebe35889" display="https://github.com/nguyentienminh07102004/product-management/commit/7bb55ddda4cb256a0125f3d907b4e273ec7230a9 - diff-4ea027d01c6e49507fa3f91d5a63f7466ff135dff36912874b4cf40bebe35889" xr:uid="{B6816B8D-E310-4C65-B7CB-4C66A0498A2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3. Danh muc san pham(tiep)
</commit_message>
<xml_diff>
--- a/product-management.xlsx
+++ b/product-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BE\MyBE\product-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB0AFD1-1951-4301-953C-D327543BD85E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7AEBDB-9CEE-4EA8-BC6D-C09F8EE15152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DDC02E0-16B2-45B2-A6F5-4A93BA49B196}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Trước bài 17</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t xml:space="preserve">2. tiny MCE base </t>
+  </si>
+  <si>
+    <t>3. Danh mục sản phẩm (Phần 1)</t>
   </si>
 </sst>
 </file>
@@ -593,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E7EC78-E1C5-4C2A-B761-4A39D954FBB0}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +821,11 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -845,8 +853,9 @@
     <hyperlink ref="C21" r:id="rId20" xr:uid="{E01490D7-8388-4F9D-83AD-E22DFD5AA4CA}"/>
     <hyperlink ref="B22" r:id="rId21" display="https://github.com/nguyentienminh07102004/product-management/commit/d0a373564e97957e32fc6716531b8809e75cba35" xr:uid="{CA423CC0-9546-4B5B-B690-3C96F405BB13}"/>
     <hyperlink ref="B23" r:id="rId22" location="diff-4ea027d01c6e49507fa3f91d5a63f7466ff135dff36912874b4cf40bebe35889" display="https://github.com/nguyentienminh07102004/product-management/commit/7bb55ddda4cb256a0125f3d907b4e273ec7230a9 - diff-4ea027d01c6e49507fa3f91d5a63f7466ff135dff36912874b4cf40bebe35889" xr:uid="{B6816B8D-E310-4C65-B7CB-4C66A0498A2A}"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://github.com/nguyentienminh07102004/product-management/commit/1fd9d226a6e73a845938d66ef4a661b05a626904" xr:uid="{D63D206C-05BD-492F-A9A8-9026F80B6B12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>